<commit_message>
GUA uptake and default dict addition
</commit_message>
<xml_diff>
--- a/plotTPD_data programs/Furfural Area_output.xlsx
+++ b/plotTPD_data programs/Furfural Area_output.xlsx
@@ -14,15 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>H2</t>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>GUA</t>
   </si>
   <si>
     <t>CO</t>
   </si>
   <si>
-    <t>Furfural</t>
+    <t>Benzene</t>
+  </si>
+  <si>
+    <t>H2</t>
   </si>
   <si>
     <t>L</t>
@@ -383,15 +389,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -402,159 +408,491 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>39631.36800601665</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>53132.58541342252</v>
+        <v>100.9031153755845</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>95138.43180464492</v>
+      </c>
+      <c r="E2">
+        <v>130.4650801285416</v>
+      </c>
+      <c r="F2">
+        <v>42348.63346193412</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>100.9031153755845</v>
+      </c>
+      <c r="D3">
+        <v>95138.43180464492</v>
+      </c>
+      <c r="E3">
+        <v>130.4650801285416</v>
+      </c>
+      <c r="F3">
+        <v>42348.63346193412</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>0.0015</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>223.034626778876</v>
+      </c>
+      <c r="D4">
+        <v>465163.2450946325</v>
+      </c>
+      <c r="E4">
+        <v>192.1888657940042</v>
+      </c>
+      <c r="F4">
+        <v>420428.1309043836</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>0.0015</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>223.034626778876</v>
+      </c>
+      <c r="D5">
+        <v>465163.2450946325</v>
+      </c>
+      <c r="E5">
+        <v>192.1888657940042</v>
+      </c>
+      <c r="F5">
+        <v>420428.1309043836</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
         <v>0.0025</v>
       </c>
-      <c r="B3">
-        <v>70994.26829026219</v>
-      </c>
-      <c r="C3">
-        <v>133944.0461453305</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>339.2788436309526</v>
+      </c>
+      <c r="D6">
+        <v>520459.7640725159</v>
+      </c>
+      <c r="E6">
+        <v>283.9560478173095</v>
+      </c>
+      <c r="F6">
+        <v>498932.5255893225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>0.0025</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>339.2788436309526</v>
+      </c>
+      <c r="D7">
+        <v>520459.7640725159</v>
+      </c>
+      <c r="E7">
+        <v>283.9560478173095</v>
+      </c>
+      <c r="F7">
+        <v>498932.5255893225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
         <v>0.005</v>
       </c>
-      <c r="B4">
-        <v>91933.09314511133</v>
-      </c>
-      <c r="C4">
-        <v>226018.1992820919</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>465.1807271000569</v>
+      </c>
+      <c r="D8">
+        <v>620114.1085123157</v>
+      </c>
+      <c r="E8">
+        <v>360.1786409020218</v>
+      </c>
+      <c r="F8">
+        <v>588481.0315602918</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>0.005</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>465.1807271000569</v>
+      </c>
+      <c r="D9">
+        <v>620114.1085123157</v>
+      </c>
+      <c r="E9">
+        <v>360.1786409020218</v>
+      </c>
+      <c r="F9">
+        <v>588481.0315602918</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
+        <v>0.0075</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>394.7961739130043</v>
+      </c>
+      <c r="D10">
+        <v>633449.6597721943</v>
+      </c>
+      <c r="E10">
+        <v>473.2321595798624</v>
+      </c>
+      <c r="F10">
+        <v>625394.7784060101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>0.0075</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>394.7961739130043</v>
+      </c>
+      <c r="D11">
+        <v>633449.6597721943</v>
+      </c>
+      <c r="E11">
+        <v>473.2321595798624</v>
+      </c>
+      <c r="F11">
+        <v>625394.7784060101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
         <v>0.01</v>
       </c>
-      <c r="B5">
-        <v>143378.0156110354</v>
-      </c>
-      <c r="C5">
-        <v>369737.5809345616</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="B6">
-        <v>194360.4783134974</v>
-      </c>
-      <c r="C6">
-        <v>552878.0882018403</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="B7">
-        <v>220179.738802942</v>
-      </c>
-      <c r="C7">
-        <v>629647.1761654048</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="B8">
-        <v>234652.3982098907</v>
-      </c>
-      <c r="C8">
-        <v>689375.7473652598</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>646.5509007383389</v>
+      </c>
+      <c r="D12">
+        <v>679197.1126358224</v>
+      </c>
+      <c r="E12">
+        <v>678.2527786615456</v>
+      </c>
+      <c r="F12">
+        <v>697956.9060251359</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>646.5509007383389</v>
+      </c>
+      <c r="D13">
+        <v>679197.1126358224</v>
+      </c>
+      <c r="E13">
+        <v>678.2527786615456</v>
+      </c>
+      <c r="F13">
+        <v>697956.9060251359</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>0.015</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>771.9062671769528</v>
+      </c>
+      <c r="D14">
+        <v>719467.2486597623</v>
+      </c>
+      <c r="E14">
+        <v>827.265104584761</v>
+      </c>
+      <c r="F14">
+        <v>734678.1828283533</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1">
+        <v>0.015</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>771.9062671769528</v>
+      </c>
+      <c r="D15">
+        <v>719467.2486597623</v>
+      </c>
+      <c r="E15">
+        <v>827.265104584761</v>
+      </c>
+      <c r="F15">
+        <v>734678.1828283533</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
+        <v>0.025</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>772.3893907209838</v>
+      </c>
+      <c r="D16">
+        <v>716449.0915757268</v>
+      </c>
+      <c r="E16">
+        <v>1040.291331879298</v>
+      </c>
+      <c r="F16">
+        <v>730688.6440168284</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>0.025</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>772.3893907209838</v>
+      </c>
+      <c r="D17">
+        <v>716449.0915757268</v>
+      </c>
+      <c r="E17">
+        <v>1040.291331879298</v>
+      </c>
+      <c r="F17">
+        <v>730688.6440168284</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>0.035</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>938.0828206807664</v>
+      </c>
+      <c r="D18">
+        <v>715231.6991175624</v>
+      </c>
+      <c r="E18">
+        <v>1033.295247007901</v>
+      </c>
+      <c r="F18">
+        <v>731480.641309642</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>0.035</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>938.0828206807664</v>
+      </c>
+      <c r="D19">
+        <v>715231.6991175624</v>
+      </c>
+      <c r="E19">
+        <v>1033.295247007901</v>
+      </c>
+      <c r="F19">
+        <v>731480.641309642</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1">
         <v>0.05</v>
       </c>
-      <c r="B9">
-        <v>247006.0051625102</v>
-      </c>
-      <c r="C9">
-        <v>713826.6377626053</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="B10">
-        <v>246696.0825926914</v>
-      </c>
-      <c r="C10">
-        <v>736556.9853080336</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="B11">
-        <v>226920.0457996936</v>
-      </c>
-      <c r="C11">
-        <v>674274.0759743322</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="B12">
-        <v>247376.3455212875</v>
-      </c>
-      <c r="C12">
-        <v>722839.7213749806</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>751.507102560797</v>
+      </c>
+      <c r="D20">
+        <v>711438.0454169901</v>
+      </c>
+      <c r="E20">
+        <v>1150.511324432135</v>
+      </c>
+      <c r="F20">
+        <v>739984.1634050561</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>751.507102560797</v>
+      </c>
+      <c r="D21">
+        <v>711438.0454169901</v>
+      </c>
+      <c r="E21">
+        <v>1150.511324432135</v>
+      </c>
+      <c r="F21">
+        <v>739984.1634050561</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>703.8870880934717</v>
+      </c>
+      <c r="D22">
+        <v>716228.5907921764</v>
+      </c>
+      <c r="E22">
+        <v>1201.937726251009</v>
+      </c>
+      <c r="F22">
+        <v>726360.8306834709</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>703.8870880934717</v>
+      </c>
+      <c r="D23">
+        <v>716228.5907921764</v>
+      </c>
+      <c r="E23">
+        <v>1201.937726251009</v>
+      </c>
+      <c r="F23">
+        <v>726360.8306834709</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>1042.314641910106</v>
+      </c>
+      <c r="D24">
+        <v>718842.1125795704</v>
+      </c>
+      <c r="E24">
+        <v>1152.24018865904</v>
+      </c>
+      <c r="F24">
+        <v>745619.142100472</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>1042.314641910106</v>
+      </c>
+      <c r="D25">
+        <v>718842.1125795704</v>
+      </c>
+      <c r="E25">
+        <v>1152.24018865904</v>
+      </c>
+      <c r="F25">
+        <v>745619.142100472</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
furfural additions and calibration values for MB chamber
</commit_message>
<xml_diff>
--- a/plotTPD_data programs/Furfural Area_output.xlsx
+++ b/plotTPD_data programs/Furfural Area_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>H2</t>
   </si>
@@ -31,31 +31,13 @@
     <t>Propylene</t>
   </si>
   <si>
+    <t>CO2</t>
+  </si>
+  <si>
     <t>Furan</t>
   </si>
   <si>
-    <t>Me-furan</t>
-  </si>
-  <si>
     <t>Furfural</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>27-eth</t>
-  </si>
-  <si>
-    <t>Formaldehyde</t>
-  </si>
-  <si>
-    <t>31-ol</t>
-  </si>
-  <si>
-    <t>CO2</t>
   </si>
   <si>
     <t>L</t>
@@ -416,15 +398,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -450,37 +432,19 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>204938.5981230211</v>
+        <v>6.816250324477081e-07</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>797747.951235926</v>
+        <v>2.482357144053704e-07</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -495,39 +459,21 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>125480.2552661028</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>1.393672786043403e-08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
-        <v>3</v>
+        <v>0.1</v>
       </c>
       <c r="B3">
-        <v>282931.7183127304</v>
+        <v>5.042037834380973e-06</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>797747.951235926</v>
+        <v>8.540161573218964e-06</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -542,39 +488,21 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>432555.64615211</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <v>2.500791439450045e-07</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
-        <v>3.7</v>
+        <v>0.13</v>
       </c>
       <c r="B4">
-        <v>273302.7121123575</v>
+        <v>3.948567804934743e-06</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>797747.951235926</v>
+        <v>8.536543819799699e-06</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -589,39 +517,21 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>379325.5319329025</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+        <v>1.688194100535006e-07</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
-        <v>4.5</v>
+        <v>0.14</v>
       </c>
       <c r="B5">
-        <v>336408.3379360895</v>
+        <v>4.326178548097709e-06</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>630280.4562737856</v>
+        <v>8.228839267766388e-06</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -636,25 +546,181 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>1490170.984516413</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
+        <v>1.629888041917496e-07</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="B6">
+        <v>4.416724901953071e-06</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1.015107193083668e-05</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1.627609185457209e-06</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="B7">
+        <v>5.984335267943471e-06</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1.00470243674512e-05</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>9.040823630529e-07</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="B8">
+        <v>4.235344059260807e-06</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>8.603776128560917e-06</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1.48708086255239e-06</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="B9">
+        <v>5.910972037532766e-06</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>9.757075148098375e-06</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>2.242190889275795e-06</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="B10">
+        <v>6.299399625066266e-06</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>9.947856412959329e-06</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>5.601783900947085e-06</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="B11">
+        <v>5.698042827738062e-06</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1.020873319628905e-05</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1.067070616534278e-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>